<commit_message>
media e desvio padrão
</commit_message>
<xml_diff>
--- a/agentes.xlsx
+++ b/agentes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brenda\Desktop\escape-da-enchente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBEA2E32-6814-40D7-9A7B-73A48A71BE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBDB32E-9F66-44A2-B5DA-12D229DBCCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F569ED1-4204-47D2-8E86-06391C1C191E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="12">
   <si>
     <t>7,5 metros</t>
   </si>
@@ -67,18 +67,35 @@
   <si>
     <t>13,5 metros</t>
   </si>
+  <si>
+    <t>média</t>
+  </si>
+  <si>
+    <t>desvio padrão</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +118,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,14 +436,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8572D400-837F-47ED-99A9-06CE3C6AD5C5}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -857,441 +877,625 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B3:B12)</f>
+        <v>21.8</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C3:C12)</f>
+        <v>43.4</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D3:D12)</f>
+        <v>76.099999999999994</v>
+      </c>
+      <c r="G13">
+        <f>AVERAGE(G3:G12)</f>
+        <v>18.8</v>
+      </c>
+      <c r="H13">
+        <f>AVERAGE(H3:H12)</f>
+        <v>39.5</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(I3:I12)</f>
+        <v>73.599999999999994</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="L13:N13" si="0">AVERAGE(L3:L12)</f>
+        <v>19.2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>33.1</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="2">
+        <f>STDEV(B3:B12)</f>
+        <v>2.2509257354845511</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:N14" si="1">STDEV(C3:C12)</f>
+        <v>1.8973665961010278</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6633299933166197</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <f>STDEV(G3:G12)</f>
+        <v>1.2292725943057181</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5811388300841898</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3664319132398464</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2292725943057181</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0789954839350235</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6193277068654826</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>8</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>1</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L17" t="s">
         <v>9</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M17" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G18" t="s">
         <v>2</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H18" t="s">
         <v>3</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I18" t="s">
         <v>4</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L18" t="s">
         <v>2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M18" t="s">
         <v>3</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N18" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>34</v>
-      </c>
-      <c r="D17">
-        <v>65</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>22</v>
-      </c>
-      <c r="H17">
-        <v>39</v>
-      </c>
-      <c r="I17">
-        <v>76</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>22</v>
-      </c>
-      <c r="M17">
-        <v>41</v>
-      </c>
-      <c r="N17">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>18</v>
-      </c>
-      <c r="C18">
-        <v>30</v>
-      </c>
-      <c r="D18">
-        <v>66</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>21</v>
-      </c>
-      <c r="H18">
-        <v>35</v>
-      </c>
-      <c r="I18">
-        <v>73</v>
-      </c>
-      <c r="K18">
-        <v>2</v>
-      </c>
-      <c r="L18">
-        <v>21</v>
-      </c>
-      <c r="M18">
-        <v>40</v>
-      </c>
-      <c r="N18">
-        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I19">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M19">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N19">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H20">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L20">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M20">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N20">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>70</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>33</v>
+      </c>
+      <c r="I21">
+        <v>77</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
         <v>19</v>
       </c>
-      <c r="C21">
-        <v>30</v>
-      </c>
-      <c r="D21">
-        <v>68</v>
-      </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
-      </c>
-      <c r="H21">
-        <v>34</v>
-      </c>
-      <c r="I21">
-        <v>69</v>
-      </c>
-      <c r="K21">
-        <v>5</v>
-      </c>
-      <c r="L21">
-        <v>21</v>
-      </c>
       <c r="M21">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N21">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D22">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <v>19</v>
       </c>
       <c r="H22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I22">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="K22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L22">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M22">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="N22">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>34</v>
+      </c>
+      <c r="I23">
+        <v>69</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+      <c r="L23">
         <v>21</v>
       </c>
-      <c r="C23">
-        <v>33</v>
-      </c>
-      <c r="D23">
-        <v>67</v>
-      </c>
-      <c r="F23">
-        <v>7</v>
-      </c>
-      <c r="G23">
-        <v>22</v>
-      </c>
-      <c r="H23">
+      <c r="M23">
         <v>39</v>
       </c>
-      <c r="I23">
-        <v>74</v>
-      </c>
-      <c r="K23">
-        <v>7</v>
-      </c>
-      <c r="L23">
-        <v>19</v>
-      </c>
-      <c r="M23">
-        <v>42</v>
-      </c>
       <c r="N23">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>18</v>
       </c>
       <c r="C24">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H24">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I24">
+        <v>71</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>19</v>
+      </c>
+      <c r="M24">
+        <v>41</v>
+      </c>
+      <c r="N24">
         <v>77</v>
-      </c>
-      <c r="K24">
-        <v>8</v>
-      </c>
-      <c r="L24">
-        <v>20</v>
-      </c>
-      <c r="M24">
-        <v>40</v>
-      </c>
-      <c r="N24">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B25">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>33</v>
       </c>
       <c r="D25">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G25">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H25">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="I25">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K25">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L25">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M25">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N25">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>69</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+      <c r="H26">
+        <v>37</v>
+      </c>
+      <c r="I26">
+        <v>77</v>
+      </c>
+      <c r="K26">
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <v>20</v>
+      </c>
+      <c r="M26">
+        <v>40</v>
+      </c>
+      <c r="N26">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>68</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>35</v>
+      </c>
+      <c r="I27">
+        <v>75</v>
+      </c>
+      <c r="K27">
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <v>22</v>
+      </c>
+      <c r="M27">
+        <v>44</v>
+      </c>
+      <c r="N27">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>10</v>
       </c>
-      <c r="B26">
+      <c r="B28">
         <v>20</v>
       </c>
-      <c r="C26">
+      <c r="C28">
         <v>32</v>
       </c>
-      <c r="D26">
+      <c r="D28">
         <v>66</v>
       </c>
-      <c r="F26">
+      <c r="F28">
         <v>10</v>
       </c>
-      <c r="G26">
+      <c r="G28">
         <v>20</v>
       </c>
-      <c r="H26">
+      <c r="H28">
         <v>38</v>
       </c>
-      <c r="I26">
+      <c r="I28">
         <v>73</v>
       </c>
-      <c r="K26">
+      <c r="K28">
         <v>10</v>
       </c>
-      <c r="L26">
+      <c r="L28">
         <v>21</v>
       </c>
-      <c r="M26">
+      <c r="M28">
         <v>43</v>
       </c>
-      <c r="N26">
+      <c r="N28">
         <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <f>AVERAGE(B19:B28)</f>
+        <v>19.2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:E29" si="2">AVERAGE(C19:C28)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>67.400000000000006</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:H29" si="3">AVERAGE(G19:G28)</f>
+        <v>21.2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>36.1</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29" si="4">AVERAGE(I19:I28)</f>
+        <v>74</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29" si="5">AVERAGE(L19:L28)</f>
+        <v>20.7</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ref="M29" si="6">AVERAGE(M19:M28)</f>
+        <v>41.7</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29" si="7">AVERAGE(N19:N28)</f>
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <f>STDEV(B19:B28)</f>
+        <v>1.0327955589886444</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:N30" si="8">STDEV(C19:C28)</f>
+        <v>1.8408935028645435</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="8"/>
+        <v>1.646545204697129</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="8"/>
+        <v>1.6193277068654823</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="8"/>
+        <v>2.0789954839350235</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="8"/>
+        <v>2.5819888974716112</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="8"/>
+        <v>1.4181364924121764</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="8"/>
+        <v>1.7669811040931427</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="8"/>
+        <v>1.3703203194062976</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005175A8CD9587634B938D577990AADA98" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7cd180f61d765a255f14d21c472bc962">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e7c0ff8-d6f3-4c26-8f31-7d852eb20058" xmlns:ns4="beb6920f-0b11-4754-8fb0-f06898363c6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b12345916f391d7dde69cfd680f42b29" ns3:_="" ns4:_="">
     <xsd:import namespace="5e7c0ff8-d6f3-4c26-8f31-7d852eb20058"/>
@@ -1520,22 +1724,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0771E72-8DF0-471A-96E0-9A82844AD493}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="beb6920f-0b11-4754-8fb0-f06898363c6b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5e7c0ff8-d6f3-4c26-8f31-7d852eb20058"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C8F4079-3764-41E1-A870-147F7DFBF3A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BD564AE-53F7-46E4-8F68-55B112FF36CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1552,29 +1766,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C8F4079-3764-41E1-A870-147F7DFBF3A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0771E72-8DF0-471A-96E0-9A82844AD493}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="beb6920f-0b11-4754-8fb0-f06898363c6b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5e7c0ff8-d6f3-4c26-8f31-7d852eb20058"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>